<commit_message>
chore(exportDoc): add role column to exported excel sheet
- add staffRole to the list of eager loaded models
- update claim filter function to include role
- update excel headers to include role

[Finishes #164681727]
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
   <si>
     <t>S/N</t>
   </si>
@@ -28,6 +28,9 @@
     <t>MiddleName</t>
   </si>
   <si>
+    <t>Role</t>
+  </si>
+  <si>
     <t>Branch</t>
   </si>
   <si>
@@ -64,6 +67,9 @@
     <t>Pitz</t>
   </si>
   <si>
+    <t>Service Executive (Financial)</t>
+  </si>
+  <si>
     <t>Oyin Jolayemi</t>
   </si>
   <si>
@@ -104,6 +110,9 @@
   </si>
   <si>
     <t>Zulch</t>
+  </si>
+  <si>
+    <t>Service Executive (Non-Financial)</t>
   </si>
   <si>
     <t>Cancelled</t>
@@ -483,13 +492,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="13" width="10" customWidth="1"/>
+    <col min="1" max="14" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -529,119 +538,131 @@
       <c r="M1" t="s">
         <v>12</v>
       </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2">
-        <v>16</v>
-      </c>
-      <c r="I2">
+      <c r="J2">
         <v>5</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>6400</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
       <c r="M2" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H3">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
         <v>20</v>
       </c>
       <c r="I3">
+        <v>20</v>
+      </c>
+      <c r="J3">
         <v>8</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>9400</v>
       </c>
-      <c r="L3" t="s">
-        <v>25</v>
-      </c>
       <c r="M3" t="s">
-        <v>26</v>
+        <v>27</v>
+      </c>
+      <c r="N3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="D4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I4">
         <v>9</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>2</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <v>2950</v>
       </c>
-      <c r="L4" t="s">
-        <v>31</v>
-      </c>
       <c r="M4" t="s">
-        <v>20</v>
+        <v>34</v>
+      </c>
+      <c r="N4" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>